<commit_message>
Login functionality regression tests
</commit_message>
<xml_diff>
--- a/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
+++ b/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatevik.navasardyan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\QualisAutomationProject\WebAutomationModule\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FC2A8F5-1300-48BC-A6E6-79472BA9980D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F8268-8BED-4626-8394-08D55223FAB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>superuser</t>
   </si>
@@ -78,13 +78,128 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>qataskdemoaccnt@gmail.com</t>
+  </si>
+  <si>
+    <t>!Qualis1_1</t>
+  </si>
+  <si>
+    <t>forgot password user</t>
+  </si>
+  <si>
+    <t>newPT_686*861</t>
+  </si>
+  <si>
+    <t>newPT_48*378</t>
+  </si>
+  <si>
+    <t>newPT_520*504</t>
+  </si>
+  <si>
+    <t>newPT_252*57</t>
+  </si>
+  <si>
+    <t>newPT_568*475</t>
+  </si>
+  <si>
+    <t>newPT_162*439</t>
+  </si>
+  <si>
+    <t>newPT_727*543</t>
+  </si>
+  <si>
+    <t>newPT_633*817</t>
+  </si>
+  <si>
+    <t>newPT_905*616</t>
+  </si>
+  <si>
+    <t>newPT_256*73</t>
+  </si>
+  <si>
+    <t>newPT_408*677</t>
+  </si>
+  <si>
+    <t>newPT_442*516</t>
+  </si>
+  <si>
+    <t>newPT_599*278</t>
+  </si>
+  <si>
+    <t>newPT_845*95</t>
+  </si>
+  <si>
+    <t>newPT_262*440</t>
+  </si>
+  <si>
+    <t>newPT_269*53</t>
+  </si>
+  <si>
+    <t>newPT_572*424</t>
+  </si>
+  <si>
+    <t>newPT_774*594</t>
+  </si>
+  <si>
+    <t>newPT_166*511</t>
+  </si>
+  <si>
+    <t>newPT_649*553</t>
+  </si>
+  <si>
+    <t>newPT_273*198</t>
+  </si>
+  <si>
+    <t>newPT_423*298</t>
+  </si>
+  <si>
+    <t>newPT_336*323</t>
+  </si>
+  <si>
+    <t>newPT_737*553</t>
+  </si>
+  <si>
+    <t>newPT_23*62</t>
+  </si>
+  <si>
+    <t>newPT_322*443</t>
+  </si>
+  <si>
+    <t>newPT_188*235</t>
+  </si>
+  <si>
+    <t>newPT_768*906</t>
+  </si>
+  <si>
+    <t>newPT_32*113</t>
+  </si>
+  <si>
+    <t>newPT_354*652</t>
+  </si>
+  <si>
+    <t>newPT_873*420</t>
+  </si>
+  <si>
+    <t>newPT_46*79</t>
+  </si>
+  <si>
+    <t>newPT_135*618</t>
+  </si>
+  <si>
+    <t>newPT_910*811</t>
+  </si>
+  <si>
+    <t>newPT_407*602</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +214,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,9 +243,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,20 +566,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="36.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -463,7 +591,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -474,7 +602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -485,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -496,7 +624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -505,43 +633,55 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{379DC6A0-06B3-46F7-A699-24DC37BD2B1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding bitbucket pipeline yml file
</commit_message>
<xml_diff>
--- a/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
+++ b/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>superuser</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>newPT_357*534</t>
+  </si>
+  <si>
+    <t>newPT_665*681</t>
   </si>
 </sst>
 </file>
@@ -646,7 +649,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change verify to clean install
</commit_message>
<xml_diff>
--- a/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
+++ b/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>superuser</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>newPT_828*38</t>
+  </si>
+  <si>
+    <t>newPT_829*363</t>
   </si>
 </sst>
 </file>
@@ -652,7 +655,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Order creation scenario along with code refactoring
</commit_message>
<xml_diff>
--- a/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
+++ b/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\QualisAutomationProject\WebAutomationModule\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QualisAutomationProject\WebAutomationModule\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F8268-8BED-4626-8394-08D55223FAB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72452511-4628-457D-8214-17FA980FD2AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>superuser</t>
   </si>
@@ -47,9 +47,6 @@
     <t>autoqualisuser_opsadmin@praemium.com</t>
   </si>
   <si>
-    <t>QS@opsadminPSS123!</t>
-  </si>
-  <si>
     <t>opsadmin</t>
   </si>
   <si>
@@ -83,127 +80,52 @@
     <t>qataskdemoaccnt@gmail.com</t>
   </si>
   <si>
-    <t>!Qualis1_1</t>
-  </si>
-  <si>
     <t>forgot password user</t>
   </si>
   <si>
-    <t>newPT_686*861</t>
-  </si>
-  <si>
-    <t>newPT_48*378</t>
-  </si>
-  <si>
-    <t>newPT_520*504</t>
-  </si>
-  <si>
-    <t>newPT_252*57</t>
-  </si>
-  <si>
-    <t>newPT_568*475</t>
-  </si>
-  <si>
-    <t>newPT_162*439</t>
-  </si>
-  <si>
-    <t>newPT_727*543</t>
-  </si>
-  <si>
-    <t>newPT_633*817</t>
-  </si>
-  <si>
-    <t>newPT_905*616</t>
-  </si>
-  <si>
-    <t>newPT_256*73</t>
-  </si>
-  <si>
-    <t>newPT_408*677</t>
-  </si>
-  <si>
-    <t>newPT_442*516</t>
-  </si>
-  <si>
-    <t>newPT_599*278</t>
-  </si>
-  <si>
-    <t>newPT_845*95</t>
-  </si>
-  <si>
-    <t>newPT_262*440</t>
-  </si>
-  <si>
-    <t>newPT_269*53</t>
-  </si>
-  <si>
-    <t>newPT_572*424</t>
-  </si>
-  <si>
-    <t>newPT_774*594</t>
-  </si>
-  <si>
-    <t>newPT_166*511</t>
-  </si>
-  <si>
-    <t>newPT_649*553</t>
-  </si>
-  <si>
-    <t>newPT_273*198</t>
-  </si>
-  <si>
-    <t>newPT_423*298</t>
-  </si>
-  <si>
-    <t>newPT_336*323</t>
-  </si>
-  <si>
-    <t>newPT_737*553</t>
-  </si>
-  <si>
-    <t>newPT_23*62</t>
-  </si>
-  <si>
-    <t>newPT_322*443</t>
-  </si>
-  <si>
-    <t>newPT_188*235</t>
-  </si>
-  <si>
-    <t>newPT_768*906</t>
-  </si>
-  <si>
-    <t>newPT_32*113</t>
-  </si>
-  <si>
-    <t>newPT_354*652</t>
-  </si>
-  <si>
-    <t>newPT_873*420</t>
-  </si>
-  <si>
-    <t>newPT_46*79</t>
-  </si>
-  <si>
-    <t>newPT_135*618</t>
-  </si>
-  <si>
-    <t>newPT_910*811</t>
-  </si>
-  <si>
-    <t>newPT_407*602</t>
-  </si>
-  <si>
-    <t>newPT_357*534</t>
-  </si>
-  <si>
-    <t>newPT_665*681</t>
-  </si>
-  <si>
-    <t>newPT_828*38</t>
-  </si>
-  <si>
-    <t>newPT_829*363</t>
+    <t>!Qualis1!</t>
+  </si>
+  <si>
+    <t>fund manager</t>
+  </si>
+  <si>
+    <t>autofundmanager@praemium.com</t>
+  </si>
+  <si>
+    <t>QS@fundManagerPSS123!</t>
+  </si>
+  <si>
+    <t>newPT_787*443</t>
+  </si>
+  <si>
+    <t>invalid user</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>pass12345!.</t>
+  </si>
+  <si>
+    <t>newPT_563*42</t>
+  </si>
+  <si>
+    <t>newPT_52*371</t>
+  </si>
+  <si>
+    <t>newPT_454*815</t>
+  </si>
+  <si>
+    <t>newPT_209*822</t>
+  </si>
+  <si>
+    <t>newPT_420*269</t>
+  </si>
+  <si>
+    <t>newPT_724*740</t>
+  </si>
+  <si>
+    <t>newPT_638*235</t>
   </si>
 </sst>
 </file>
@@ -211,7 +133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,12 +148,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -255,15 +171,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -579,83 +489,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="36.109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>56</v>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -663,10 +595,10 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B6" r:id="rId7" xr:uid="{379DC6A0-06B3-46F7-A699-24DC37BD2B1B}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{379DC6A0-06B3-46F7-A699-24DC37BD2B1B}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{8D7A727B-A6E4-4D71-AF50-B73E0BA885E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId8"/>
@@ -679,7 +611,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -693,7 +625,7 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Connected to the Database.
</commit_message>
<xml_diff>
--- a/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
+++ b/WebAutomationModule/src/main/resources/qualis_users_credentials.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\QualisAutomationProject\WebAutomationModule\src\main\resources\"/>
     </mc:Choice>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>superuser</t>
   </si>
@@ -105,12 +105,22 @@
   </si>
   <si>
     <t>newPT_638*235</t>
+  </si>
+  <si>
+    <t>newPT_737*501</t>
+  </si>
+  <si>
+    <t>newPT_56*331</t>
+  </si>
+  <si>
+    <t>newPT_353*883</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,9 +485,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="36.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -543,7 +553,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>